<commit_message>
Update TS for TC003 search func 50%
</commit_message>
<xml_diff>
--- a/UC01 SearchSneakers_BossGiay_TCs.xlsx
+++ b/UC01 SearchSneakers_BossGiay_TCs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SENIUM WITH JAVA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44443A4C-6A4A-48ED-B1E4-0F9154C23F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE822D4-2CD3-4A6F-91A1-435A4A3D1ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="1" xr2:uid="{E28AEBC4-528C-4190-9FEA-BFE86C8B68D0}"/>
   </bookViews>
@@ -915,41 +915,8 @@
     <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="9" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -962,6 +929,39 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1813,8 +1813,8 @@
   </sheetPr>
   <dimension ref="A1:AU197"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H101" sqref="H101"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30:E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" outlineLevelRow="1"/>
@@ -1842,28 +1842,28 @@
     </row>
     <row r="2" spans="1:13" s="8" customFormat="1" ht="24.6">
       <c r="A2" s="11"/>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
       <c r="H2" s="12"/>
       <c r="M2" s="13"/>
     </row>
     <row r="3" spans="1:13" s="8" customFormat="1" ht="22.8">
       <c r="A3" s="11"/>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="47"/>
+      <c r="C3" s="59"/>
       <c r="D3" s="14"/>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="48"/>
+      <c r="G3" s="60"/>
       <c r="I3" s="14"/>
       <c r="J3" s="15"/>
       <c r="M3" s="13"/>
@@ -1872,11 +1872,11 @@
       <c r="A5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
@@ -1890,11 +1890,11 @@
       <c r="A6" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
@@ -1908,11 +1908,11 @@
       <c r="A7" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
       <c r="E7"/>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
@@ -1926,11 +1926,11 @@
       <c r="A8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
@@ -1944,11 +1944,11 @@
       <c r="A9" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
@@ -1962,11 +1962,11 @@
       <c r="A10" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="53">
+      <c r="B10" s="56">
         <v>44532</v>
       </c>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
@@ -1980,9 +1980,9 @@
       <c r="A11" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="53"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
@@ -2245,13 +2245,13 @@
       <c r="E21" s="31"/>
       <c r="F21" s="31"/>
       <c r="G21" s="31"/>
-      <c r="H21" s="54" t="s">
+      <c r="H21" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="I21" s="54"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="54"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="57"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="57"/>
     </row>
     <row r="22" spans="1:12" s="30" customFormat="1" ht="13.2">
       <c r="A22" s="32" t="s">
@@ -2295,11 +2295,11 @@
       <c r="A23" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="50" t="s">
+      <c r="B23" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="51"/>
-      <c r="D23" s="52"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="54"/>
       <c r="E23" s="34"/>
       <c r="F23" s="34"/>
       <c r="G23" s="34"/>
@@ -2312,102 +2312,102 @@
       <c r="L23" s="36"/>
     </row>
     <row r="24" spans="1:12" s="37" customFormat="1" ht="52.2" customHeight="1" outlineLevel="1">
-      <c r="A24" s="57"/>
-      <c r="B24" s="58" t="s">
+      <c r="A24" s="46"/>
+      <c r="B24" s="47" t="s">
         <v>49</v>
       </c>
       <c r="C24" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="59" t="s">
+      <c r="D24" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="E24" s="60" t="s">
+      <c r="E24" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="F24" s="49"/>
-      <c r="G24" s="55" t="s">
+      <c r="F24" s="45"/>
+      <c r="G24" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="H24" s="56"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
+      <c r="H24" s="51"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="45"/>
+      <c r="L24" s="45"/>
     </row>
     <row r="25" spans="1:12" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A25" s="57"/>
-      <c r="B25" s="58"/>
+      <c r="A25" s="46"/>
+      <c r="B25" s="47"/>
       <c r="C25" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="59"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="49"/>
-      <c r="K25" s="49"/>
-      <c r="L25" s="49"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="51"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="45"/>
+      <c r="L25" s="45"/>
     </row>
     <row r="26" spans="1:12" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A26" s="57"/>
-      <c r="B26" s="58"/>
+      <c r="A26" s="46"/>
+      <c r="B26" s="47"/>
       <c r="C26" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="59"/>
-      <c r="E26" s="60"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="56"/>
-      <c r="I26" s="49"/>
-      <c r="J26" s="49"/>
-      <c r="K26" s="49"/>
-      <c r="L26" s="49"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="51"/>
+      <c r="I26" s="45"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="45"/>
     </row>
     <row r="27" spans="1:12" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A27" s="57"/>
-      <c r="B27" s="58"/>
+      <c r="A27" s="46"/>
+      <c r="B27" s="47"/>
       <c r="C27" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="59"/>
-      <c r="E27" s="60"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="56"/>
-      <c r="I27" s="49"/>
-      <c r="J27" s="49"/>
-      <c r="K27" s="49"/>
-      <c r="L27" s="49"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="45"/>
+      <c r="L27" s="45"/>
     </row>
     <row r="28" spans="1:12" s="37" customFormat="1" ht="35.4" customHeight="1" outlineLevel="1">
-      <c r="A28" s="57"/>
-      <c r="B28" s="58"/>
+      <c r="A28" s="46"/>
+      <c r="B28" s="47"/>
       <c r="C28" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="59"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="56"/>
-      <c r="I28" s="49"/>
-      <c r="J28" s="49"/>
-      <c r="K28" s="49"/>
-      <c r="L28" s="49"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
+      <c r="K28" s="45"/>
+      <c r="L28" s="45"/>
     </row>
     <row r="29" spans="1:12" s="18" customFormat="1" ht="13.2">
       <c r="A29" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="50" t="s">
+      <c r="B29" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="51"/>
-      <c r="D29" s="52"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="54"/>
       <c r="E29" s="34"/>
       <c r="F29" s="34"/>
       <c r="G29" s="34"/>
@@ -2418,100 +2418,100 @@
       <c r="L29" s="36"/>
     </row>
     <row r="30" spans="1:12" s="37" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
-      <c r="A30" s="57"/>
-      <c r="B30" s="58" t="s">
+      <c r="A30" s="46"/>
+      <c r="B30" s="47" t="s">
         <v>49</v>
       </c>
       <c r="C30" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="D30" s="59" t="s">
+      <c r="D30" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="E30" s="60" t="s">
+      <c r="E30" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="F30" s="49"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="49"/>
-      <c r="J30" s="49"/>
-      <c r="K30" s="49"/>
-      <c r="L30" s="49"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="50"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
+      <c r="K30" s="45"/>
+      <c r="L30" s="45"/>
     </row>
     <row r="31" spans="1:12" s="37" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
-      <c r="A31" s="57"/>
-      <c r="B31" s="58"/>
+      <c r="A31" s="46"/>
+      <c r="B31" s="47"/>
       <c r="C31" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="59"/>
-      <c r="E31" s="60"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="55"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="49"/>
-      <c r="J31" s="49"/>
-      <c r="K31" s="49"/>
-      <c r="L31" s="49"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="50"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
+      <c r="K31" s="45"/>
+      <c r="L31" s="45"/>
     </row>
     <row r="32" spans="1:12" s="37" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
-      <c r="A32" s="57"/>
-      <c r="B32" s="58"/>
+      <c r="A32" s="46"/>
+      <c r="B32" s="47"/>
       <c r="C32" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="D32" s="59"/>
-      <c r="E32" s="60"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="55"/>
-      <c r="H32" s="56"/>
-      <c r="I32" s="49"/>
-      <c r="J32" s="49"/>
-      <c r="K32" s="49"/>
-      <c r="L32" s="49"/>
+      <c r="D32" s="48"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="50"/>
+      <c r="H32" s="51"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="45"/>
+      <c r="K32" s="45"/>
+      <c r="L32" s="45"/>
     </row>
     <row r="33" spans="1:47" s="37" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
-      <c r="A33" s="57"/>
-      <c r="B33" s="58"/>
+      <c r="A33" s="46"/>
+      <c r="B33" s="47"/>
       <c r="C33" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D33" s="59"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="55"/>
-      <c r="H33" s="56"/>
-      <c r="I33" s="49"/>
-      <c r="J33" s="49"/>
-      <c r="K33" s="49"/>
-      <c r="L33" s="49"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="50"/>
+      <c r="H33" s="51"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="45"/>
+      <c r="K33" s="45"/>
+      <c r="L33" s="45"/>
     </row>
     <row r="34" spans="1:47" s="37" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
-      <c r="A34" s="57"/>
-      <c r="B34" s="58"/>
+      <c r="A34" s="46"/>
+      <c r="B34" s="47"/>
       <c r="C34" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="D34" s="59"/>
-      <c r="E34" s="60"/>
-      <c r="F34" s="49"/>
-      <c r="G34" s="55"/>
-      <c r="H34" s="56"/>
-      <c r="I34" s="49"/>
-      <c r="J34" s="49"/>
-      <c r="K34" s="49"/>
-      <c r="L34" s="49"/>
+      <c r="D34" s="48"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="50"/>
+      <c r="H34" s="51"/>
+      <c r="I34" s="45"/>
+      <c r="J34" s="45"/>
+      <c r="K34" s="45"/>
+      <c r="L34" s="45"/>
     </row>
     <row r="35" spans="1:47" s="18" customFormat="1" ht="13.2">
       <c r="A35" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="50" t="s">
+      <c r="B35" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="C35" s="51"/>
-      <c r="D35" s="52"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="54"/>
       <c r="E35" s="34"/>
       <c r="F35" s="34"/>
       <c r="G35" s="34"/>
@@ -2524,92 +2524,92 @@
       <c r="L35" s="36"/>
     </row>
     <row r="36" spans="1:47" s="37" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
-      <c r="A36" s="57"/>
-      <c r="B36" s="58" t="s">
+      <c r="A36" s="46"/>
+      <c r="B36" s="47" t="s">
         <v>49</v>
       </c>
       <c r="C36" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="D36" s="59" t="s">
+      <c r="D36" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="E36" s="60" t="s">
+      <c r="E36" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="F36" s="49"/>
-      <c r="G36" s="55" t="s">
+      <c r="F36" s="45"/>
+      <c r="G36" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="H36" s="56"/>
-      <c r="I36" s="49"/>
-      <c r="J36" s="49"/>
-      <c r="K36" s="49"/>
-      <c r="L36" s="49"/>
+      <c r="H36" s="51"/>
+      <c r="I36" s="45"/>
+      <c r="J36" s="45"/>
+      <c r="K36" s="45"/>
+      <c r="L36" s="45"/>
     </row>
     <row r="37" spans="1:47" s="37" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
-      <c r="A37" s="57"/>
-      <c r="B37" s="58"/>
+      <c r="A37" s="46"/>
+      <c r="B37" s="47"/>
       <c r="C37" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="D37" s="59"/>
-      <c r="E37" s="60"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="55"/>
-      <c r="H37" s="56"/>
-      <c r="I37" s="49"/>
-      <c r="J37" s="49"/>
-      <c r="K37" s="49"/>
-      <c r="L37" s="49"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="51"/>
+      <c r="I37" s="45"/>
+      <c r="J37" s="45"/>
+      <c r="K37" s="45"/>
+      <c r="L37" s="45"/>
     </row>
     <row r="38" spans="1:47" s="37" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
-      <c r="A38" s="57"/>
-      <c r="B38" s="58"/>
+      <c r="A38" s="46"/>
+      <c r="B38" s="47"/>
       <c r="C38" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="D38" s="59"/>
-      <c r="E38" s="60"/>
-      <c r="F38" s="49"/>
-      <c r="G38" s="55"/>
-      <c r="H38" s="56"/>
-      <c r="I38" s="49"/>
-      <c r="J38" s="49"/>
-      <c r="K38" s="49"/>
-      <c r="L38" s="49"/>
+      <c r="D38" s="48"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="45"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="51"/>
+      <c r="I38" s="45"/>
+      <c r="J38" s="45"/>
+      <c r="K38" s="45"/>
+      <c r="L38" s="45"/>
     </row>
     <row r="39" spans="1:47" s="37" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
-      <c r="A39" s="57"/>
-      <c r="B39" s="58"/>
+      <c r="A39" s="46"/>
+      <c r="B39" s="47"/>
       <c r="C39" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D39" s="59"/>
-      <c r="E39" s="60"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="55"/>
-      <c r="H39" s="56"/>
-      <c r="I39" s="49"/>
-      <c r="J39" s="49"/>
-      <c r="K39" s="49"/>
-      <c r="L39" s="49"/>
+      <c r="D39" s="48"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="45"/>
+      <c r="G39" s="50"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="45"/>
+      <c r="J39" s="45"/>
+      <c r="K39" s="45"/>
+      <c r="L39" s="45"/>
     </row>
     <row r="40" spans="1:47" s="37" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
-      <c r="A40" s="57"/>
-      <c r="B40" s="58"/>
+      <c r="A40" s="46"/>
+      <c r="B40" s="47"/>
       <c r="C40" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="D40" s="59"/>
-      <c r="E40" s="60"/>
-      <c r="F40" s="49"/>
-      <c r="G40" s="55"/>
-      <c r="H40" s="56"/>
-      <c r="I40" s="49"/>
-      <c r="J40" s="49"/>
-      <c r="K40" s="49"/>
-      <c r="L40" s="49"/>
+      <c r="D40" s="48"/>
+      <c r="E40" s="49"/>
+      <c r="F40" s="45"/>
+      <c r="G40" s="50"/>
+      <c r="H40" s="51"/>
+      <c r="I40" s="45"/>
+      <c r="J40" s="45"/>
+      <c r="K40" s="45"/>
+      <c r="L40" s="45"/>
     </row>
     <row r="41" spans="1:47">
       <c r="A41" s="39"/>
@@ -10307,13 +10307,30 @@
   </sheetData>
   <autoFilter ref="A22:L22" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <mergeCells count="47">
-    <mergeCell ref="J36:J40"/>
-    <mergeCell ref="K36:K40"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="B36:B40"/>
-    <mergeCell ref="D36:D40"/>
-    <mergeCell ref="E36:E40"/>
-    <mergeCell ref="F36:F40"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="L24:L28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="H21:L21"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="G24:G28"/>
+    <mergeCell ref="H24:H28"/>
+    <mergeCell ref="I24:I28"/>
+    <mergeCell ref="J24:J28"/>
+    <mergeCell ref="K24:K28"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="D24:D28"/>
+    <mergeCell ref="E24:E28"/>
+    <mergeCell ref="F24:F28"/>
     <mergeCell ref="L36:L40"/>
     <mergeCell ref="A30:A34"/>
     <mergeCell ref="B30:B34"/>
@@ -10330,30 +10347,13 @@
     <mergeCell ref="G36:G40"/>
     <mergeCell ref="H36:H40"/>
     <mergeCell ref="I36:I40"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="D24:D28"/>
-    <mergeCell ref="E24:E28"/>
-    <mergeCell ref="F24:F28"/>
-    <mergeCell ref="L24:L28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="H21:L21"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="G24:G28"/>
-    <mergeCell ref="H24:H28"/>
-    <mergeCell ref="I24:I28"/>
-    <mergeCell ref="J24:J28"/>
-    <mergeCell ref="K24:K28"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="J36:J40"/>
+    <mergeCell ref="K36:K40"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="D36:D40"/>
+    <mergeCell ref="E36:E40"/>
+    <mergeCell ref="F36:F40"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" sqref="MFX23:MGA40 AMR23:AMU40 SHL23:SHO40 AWN23:AWQ40 MPT23:MPW40 BGJ23:BGM40 VIF23:VII40 BQF23:BQI40 MZP23:MZS40 CAB23:CAE40 SRH23:SRK40 CJX23:CKA40 NJL23:NJO40 CTT23:CTW40 WVP23:WVS40 DDP23:DDS40 NTH23:NTK40 DNL23:DNO40 TBD23:TBG40 DXH23:DXK40 ODD23:ODG40 EHD23:EHG40 VSB23:VSE40 EQZ23:ERC40 OMZ23:ONC40 FAV23:FAY40 TKZ23:TLC40 FKR23:FKU40 OWV23:OWY40 FUN23:FUQ40 JD23:JG40 GEJ23:GEM40 PGR23:PGU40 GOF23:GOI40 TUV23:TUY40 GYB23:GYE40 PQN23:PQQ40 HHX23:HIA40 WBX23:WCA40 HRT23:HRW40 QAJ23:QAM40 IBP23:IBS40 UER23:UEU40 ILL23:ILO40 QKF23:QKI40 IVH23:IVK40 SZ23:TC40 JFD23:JFG40 QUB23:QUE40 JOZ23:JPC40 UON23:UOQ40 JYV23:JYY40 RDX23:REA40 KIR23:KIU40 WLT23:WLW40 KSN23:KSQ40 RNT23:RNW40 LCJ23:LCM40 UYJ23:UYM40 LMF23:LMI40 RXP23:RXS40 LWB23:LWE40 ACV23:ACY40" xr:uid="{56D9884D-EBF1-4FBC-836F-F8753E860E4B}">

</xml_diff>